<commit_message>
Add Check list, Trst cases, updated Bug report
</commit_message>
<xml_diff>
--- a/Bug report.xlsx
+++ b/Bug report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="IT_B 1" sheetId="1" r:id="rId1"/>
@@ -30,13 +30,14 @@
     <sheet name="IT_B 22" sheetId="39" r:id="rId21"/>
     <sheet name="IT_B 23" sheetId="40" r:id="rId22"/>
     <sheet name="IT_B 24" sheetId="41" r:id="rId23"/>
+    <sheet name="IT_B 25" sheetId="42" r:id="rId24"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="138">
   <si>
     <t>Bug ID</t>
   </si>
@@ -319,10 +320,6 @@
     <t>Неполное отображение фотографий в категории portrait</t>
   </si>
   <si>
-    <t>1. Открыть главную страницу 
-2. В Header'е выбрать категорию portrait</t>
-  </si>
-  <si>
     <t>Фотографии, отображаемые на странице, соответствуют  фотографиям, отображаемым в режиме FullScreen</t>
   </si>
   <si>
@@ -446,6 +443,46 @@
   </si>
   <si>
     <t>Раздел food должен открывать страницу  с фотографиями еды</t>
+  </si>
+  <si>
+    <t>IT_B 25</t>
+  </si>
+  <si>
+    <t>1. Открыть главную страницу 
+2. Проверить расположение элементов  в  Header'е</t>
+  </si>
+  <si>
+    <t>Элементы в  Header'е должны быть расположены в определенном порядке и стиле</t>
+  </si>
+  <si>
+    <t>Расположение элемента  food  в  Header'е не соответствует общему формату</t>
+  </si>
+  <si>
+    <t>1. Открыть главную страницу 
+2. В в Footer'е кликнуть по иконке неизвестная соц сеть</t>
+  </si>
+  <si>
+    <t>1. Открыть главную страницу 
+2. В Header'е выбрать категорию portrait
+3. Просмотреть фото в обычном режиме и в режиме FullScreen</t>
+  </si>
+  <si>
+    <t>1. Открыть главную страницу 
+2. В Header'е выбрать категорию fashion
+3. Просмотреть фото в обычном режиме и в режиме FullScreen</t>
+  </si>
+  <si>
+    <t>1. Открыть главную страницу 
+2. В Header'е выбрать категорию nature
+3. Просмотреть фото в обычном режиме и в режиме FullScreen</t>
+  </si>
+  <si>
+    <t>Нет ссылки на аккаунт проекта в соц сети "ВК" в Main block на странице Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Открыть главную страницу 
+2. Перейти в раздел Contact
+3. Кликнуть по иконке соц сети "ВК" </t>
   </si>
 </sst>
 </file>
@@ -503,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -519,6 +556,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -548,7 +591,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>3209925</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>350996</xdr:rowOff>
+      <xdr:rowOff>160496</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -682,8 +725,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>3381375</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>314325</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1002,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1022,7 +1065,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" outlineLevel="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1047,7 +1090,7 @@
     </row>
     <row r="5" spans="1:2" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>19</v>
@@ -1112,7 +1155,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1156,7 +1199,7 @@
     </row>
     <row r="5" spans="1:2" ht="30" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>64</v>
@@ -1221,7 +1264,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1246,10 +1289,10 @@
       <c r="B2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" ht="30" outlineLevel="1">
       <c r="A3" s="6" t="s">
@@ -1258,8 +1301,8 @@
       <c r="B3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" outlineLevel="1">
       <c r="A4" s="6" t="s">
@@ -1268,28 +1311,28 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" outlineLevel="1">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+        <v>132</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="30" outlineLevel="1">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="30" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -1298,8 +1341,8 @@
       <c r="B7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" outlineLevel="1">
       <c r="A8" s="5" t="s">
@@ -1349,7 +1392,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1374,10 +1417,10 @@
       <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" outlineLevel="1">
       <c r="A3" s="6" t="s">
@@ -1386,8 +1429,8 @@
       <c r="B3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" outlineLevel="1">
       <c r="A4" s="6" t="s">
@@ -1396,18 +1439,18 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="30" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="45" outlineLevel="1">
       <c r="A6" s="5" t="s">
@@ -1416,8 +1459,8 @@
       <c r="B6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="60" outlineLevel="1">
       <c r="A7" s="5" t="s">
@@ -1426,8 +1469,8 @@
       <c r="B7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" outlineLevel="1">
       <c r="A8" s="5" t="s">
@@ -1469,7 +1512,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1511,7 +1554,7 @@
     </row>
     <row r="5" spans="1:2" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>78</v>
@@ -1568,7 +1611,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1610,7 +1653,7 @@
     </row>
     <row r="5" spans="1:2" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>83</v>
@@ -1675,7 +1718,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1717,12 +1760,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" outlineLevel="1">
+    <row r="5" spans="1:2" ht="60" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" outlineLevel="1">
@@ -1730,7 +1773,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="60" outlineLevel="1">
@@ -1738,7 +1781,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2" outlineLevel="1">
@@ -1776,7 +1819,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1799,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" outlineLevel="1">
@@ -1807,7 +1850,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" outlineLevel="1">
@@ -1818,12 +1861,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" outlineLevel="1">
+    <row r="5" spans="1:2" ht="60" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" outlineLevel="1">
@@ -1831,7 +1874,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" outlineLevel="1">
@@ -1839,7 +1882,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:2" outlineLevel="1">
@@ -1877,7 +1920,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -1900,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" outlineLevel="1">
@@ -1908,7 +1951,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" outlineLevel="1">
@@ -1919,12 +1962,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" outlineLevel="1">
+    <row r="5" spans="1:2" ht="60" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" outlineLevel="1">
@@ -1932,7 +1975,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" outlineLevel="1">
@@ -1940,7 +1983,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:2" outlineLevel="1">
@@ -1978,7 +2021,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2001,7 +2044,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" outlineLevel="1">
@@ -2009,7 +2052,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" outlineLevel="1">
@@ -2022,7 +2065,7 @@
     </row>
     <row r="5" spans="1:2" ht="30" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>31</v>
@@ -2033,7 +2076,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" outlineLevel="1">
@@ -2041,7 +2084,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:2" outlineLevel="1">
@@ -2079,7 +2122,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2102,22 +2145,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" ht="30" outlineLevel="1">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+        <v>100</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" outlineLevel="1">
       <c r="A4" s="6" t="s">
@@ -2126,38 +2169,38 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="60" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+        <v>101</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="30" outlineLevel="1">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+        <v>102</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="30" outlineLevel="1">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+        <v>105</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" outlineLevel="1">
       <c r="A8" s="5" t="s">
@@ -2207,7 +2250,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2251,7 +2294,7 @@
     </row>
     <row r="5" spans="1:2" ht="30" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>31</v>
@@ -2262,7 +2305,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" outlineLevel="1">
@@ -2316,7 +2359,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2339,22 +2382,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" ht="30" outlineLevel="1">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+        <v>136</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" outlineLevel="1">
       <c r="A4" s="6" t="s">
@@ -2363,38 +2406,38 @@
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="60" outlineLevel="1">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" ht="30" outlineLevel="1">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+        <v>104</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="30" outlineLevel="1">
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+        <v>105</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" outlineLevel="1">
       <c r="A8" s="5" t="s">
@@ -2425,7 +2468,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2444,7 +2487,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2465,7 +2508,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" outlineLevel="1">
@@ -2473,7 +2516,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" outlineLevel="1">
@@ -2486,10 +2529,10 @@
     </row>
     <row r="5" spans="1:2" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" outlineLevel="1">
@@ -2497,7 +2540,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" outlineLevel="1">
@@ -2505,7 +2548,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:2" outlineLevel="1">
@@ -2513,7 +2556,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2" outlineLevel="1">
@@ -2537,7 +2580,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2551,7 +2594,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2572,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" outlineLevel="1">
@@ -2580,7 +2623,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" outlineLevel="1">
@@ -2593,10 +2636,10 @@
     </row>
     <row r="5" spans="1:2" ht="60" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" outlineLevel="1">
@@ -2604,7 +2647,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" outlineLevel="1">
@@ -2612,7 +2655,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:2" outlineLevel="1">
@@ -2620,7 +2663,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:2" outlineLevel="1">
@@ -2644,7 +2687,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2658,7 +2701,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2679,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:2" outlineLevel="1">
@@ -2687,7 +2730,7 @@
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" outlineLevel="1">
@@ -2700,10 +2743,10 @@
     </row>
     <row r="5" spans="1:2" ht="75" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" outlineLevel="1">
@@ -2711,7 +2754,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" outlineLevel="1">
@@ -2719,7 +2762,114 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" outlineLevel="1">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" outlineLevel="1">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" outlineLevel="1">
+      <c r="A10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" outlineLevel="1">
+      <c r="A11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" outlineLevel="1">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" outlineLevel="1">
+      <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" outlineLevel="1">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="45" outlineLevel="1">
+      <c r="A5" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45" outlineLevel="1">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" outlineLevel="1">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:2" outlineLevel="1">
@@ -2765,7 +2915,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2809,7 +2959,7 @@
     </row>
     <row r="5" spans="1:2" ht="30" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>36</v>
@@ -2820,7 +2970,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" outlineLevel="1">
@@ -2874,7 +3024,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2918,7 +3068,7 @@
     </row>
     <row r="5" spans="1:2" ht="30" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>40</v>
@@ -2929,7 +3079,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" outlineLevel="1">
@@ -2983,7 +3133,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -3027,7 +3177,7 @@
     </row>
     <row r="5" spans="1:2" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>50</v>
@@ -3092,7 +3242,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -3136,7 +3286,7 @@
     </row>
     <row r="5" spans="1:2" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>51</v>
@@ -3201,7 +3351,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -3245,7 +3395,7 @@
     </row>
     <row r="5" spans="1:2" ht="60" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>53</v>
@@ -3310,7 +3460,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -3354,7 +3504,7 @@
     </row>
     <row r="5" spans="1:2" ht="45" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>56</v>
@@ -3419,7 +3569,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1"/>
@@ -3463,7 +3613,7 @@
     </row>
     <row r="5" spans="1:2" ht="60" outlineLevel="1">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>60</v>

</xml_diff>